<commit_message>
Initial Azure AD "New User" logic implemented.
</commit_message>
<xml_diff>
--- a/personas.xlsx
+++ b/personas.xlsx
@@ -8,24 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyler\Development\smartterhealth\content-personas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52538F2D-D0FD-44CE-AA61-B55B1F3598C6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3E136C-2232-4F0C-A3B6-250EAAD89427}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12990" xr2:uid="{87C741E5-9606-4A4F-9009-1E4112E4DF41}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="personas" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>FirstName</t>
   </si>
@@ -79,13 +85,73 @@
   </si>
   <si>
     <t>Dr. Watt</t>
+  </si>
+  <si>
+    <t>JobTitle</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Trauma Care</t>
+  </si>
+  <si>
+    <t>Office</t>
+  </si>
+  <si>
+    <t>Building 1</t>
+  </si>
+  <si>
+    <t>Nancy</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Nurse Nancy</t>
+  </si>
+  <si>
+    <t>Building 2</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Nashville</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>Radiology</t>
+  </si>
+  <si>
+    <t>AccountEnabled</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>ENTERPRISEPREMIUM;EMSPREMIUM</t>
+  </si>
+  <si>
+    <t>Office365Plans</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,16 +159,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -110,15 +189,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -139,16 +236,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A05BCBD-9362-4444-B6D3-C1287FB470BC}" name="Table1" displayName="Table1" ref="A1:F4" totalsRowShown="0">
-  <autoFilter ref="A1:F4" xr:uid="{F11B011F-1E1B-4583-908A-0C59183AED54}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{236BF943-7CEB-4C17-8BA7-42A7146DF91F}" name="Alias" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A05BCBD-9362-4444-B6D3-C1287FB470BC}" name="Table1" displayName="Table1" ref="A1:M5" totalsRowShown="0">
+  <autoFilter ref="A1:M5" xr:uid="{F11B011F-1E1B-4583-908A-0C59183AED54}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{236BF943-7CEB-4C17-8BA7-42A7146DF91F}" name="Alias" dataDxfId="0" dataCellStyle="Calculation">
       <calculatedColumnFormula>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{6FCDF76C-45C2-4AB8-8CC1-20BA4C805A59}" name="Title"/>
     <tableColumn id="2" xr3:uid="{E62E75CD-5A0E-4B86-AF35-B991CBE33DD8}" name="FirstName"/>
     <tableColumn id="3" xr3:uid="{4B996375-CD17-402D-8BEB-D35A4E982B2E}" name="LastName"/>
     <tableColumn id="6" xr3:uid="{4261D67B-BCA8-4DC2-BA94-7E9D8E51AEDD}" name="DisplayName"/>
+    <tableColumn id="8" xr3:uid="{9A0DF3BC-30FC-4022-B66D-3D4FEF34CCF1}" name="JobTitle"/>
+    <tableColumn id="9" xr3:uid="{0454B832-5924-4E24-92DC-9D0F8248A5C2}" name="Department"/>
+    <tableColumn id="5" xr3:uid="{2AC59C68-094C-4C75-8924-EACAA4C72BD1}" name="Office"/>
+    <tableColumn id="10" xr3:uid="{70A0FA65-7F00-43A2-AA4C-70B8DBDE75A6}" name="City"/>
+    <tableColumn id="11" xr3:uid="{285F77D6-2A79-4307-9E56-8B2611B6C5DA}" name="State"/>
+    <tableColumn id="13" xr3:uid="{53E7A27A-826C-4261-9349-F14D4C12AB2A}" name="Office365Plans"/>
+    <tableColumn id="12" xr3:uid="{B514E4A6-C6AC-4889-898A-AA1A53287E36}" name="AccountEnabled"/>
     <tableColumn id="4" xr3:uid="{76BA5797-6ED4-4FAD-AD0D-BDB4873AFC64}" name="UsageLocation"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -452,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA39548C-6792-479F-B44E-E97CE90FF367}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,11 +567,11 @@
     <col min="1" max="2" width="22.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="5" max="12" width="22.42578125" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -484,11 +588,32 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>drstrange</v>
       </c>
@@ -505,11 +630,32 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>drwatt</v>
       </c>
@@ -526,11 +672,32 @@
         <v>17</v>
       </c>
       <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="str">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>nursejazz</v>
       </c>
@@ -547,13 +714,77 @@
         <v>16</v>
       </c>
       <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="str">
+        <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
+        <v>nursesmith</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Started export of SPO
</commit_message>
<xml_diff>
--- a/personas.xlsx
+++ b/personas.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyler\Development\smartterhealth\content-personas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3E136C-2232-4F0C-A3B6-250EAAD89427}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9167CF-247A-4202-877D-EAD99E26990E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12990" xr2:uid="{87C741E5-9606-4A4F-9009-1E4112E4DF41}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12990" activeTab="1" xr2:uid="{87C741E5-9606-4A4F-9009-1E4112E4DF41}"/>
   </bookViews>
   <sheets>
-    <sheet name="personas" sheetId="1" r:id="rId1"/>
+    <sheet name="inputs" sheetId="2" r:id="rId1"/>
+    <sheet name="personas" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="Office365Plans">GlobalInputs[Value]</definedName>
+  </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>FirstName</t>
   </si>
@@ -145,13 +149,40 @@
   </si>
   <si>
     <t>Office365Plans</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>SPS-Skills</t>
+  </si>
+  <si>
+    <t>Hospital Medicine;Hospital Management;Outcomes Research;Teaching;Strategic Planning;EMR;Innovation</t>
+  </si>
+  <si>
+    <t>Cardiopulmonary Physical Therapy;Heat Illness Prevention;CITI Program - Human Subject Research</t>
+  </si>
+  <si>
+    <t>SPS-School</t>
+  </si>
+  <si>
+    <t>Vanderbilt University School of Medicine;University of Tennessee - Knoxville</t>
+  </si>
+  <si>
+    <t>Surgery;Cancer Treatment;Radiation Treatment;Clinical Trails;Chemotherapy</t>
+  </si>
+  <si>
+    <t>Baylor University;John Hopkins University</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,8 +198,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +223,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
       </patternFill>
     </fill>
   </fills>
@@ -205,20 +260,59 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Accent6" xfId="3" builtinId="49"/>
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF7F7F7F"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF7F7F7F"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF7F7F7F"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF7F7F7F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -236,10 +330,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A05BCBD-9362-4444-B6D3-C1287FB470BC}" name="Table1" displayName="Table1" ref="A1:M5" totalsRowShown="0">
-  <autoFilter ref="A1:M5" xr:uid="{F11B011F-1E1B-4583-908A-0C59183AED54}"/>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{236BF943-7CEB-4C17-8BA7-42A7146DF91F}" name="Alias" dataDxfId="0" dataCellStyle="Calculation">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EE6B63CB-DF51-44B2-B6E1-268D302375BC}" name="GlobalInputs" displayName="GlobalInputs" ref="B2:C3" totalsRowShown="0">
+  <autoFilter ref="B2:C3" xr:uid="{51B885EE-B54A-4B22-8BBE-6A24E37364BA}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{13495667-CD26-47D2-852E-FE8A0243D3F3}" name="Input" dataCellStyle="Good"/>
+    <tableColumn id="2" xr3:uid="{1CA1CBF2-D93F-4341-A6C1-6E4D4F42645E}" name="Value" dataDxfId="2" dataCellStyle="Accent6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A05BCBD-9362-4444-B6D3-C1287FB470BC}" name="Table1" displayName="Table1" ref="A1:O5" totalsRowShown="0">
+  <autoFilter ref="A1:O5" xr:uid="{F11B011F-1E1B-4583-908A-0C59183AED54}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{236BF943-7CEB-4C17-8BA7-42A7146DF91F}" name="Alias" dataDxfId="3" dataCellStyle="Calculation">
       <calculatedColumnFormula>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{6FCDF76C-45C2-4AB8-8CC1-20BA4C805A59}" name="Title"/>
@@ -251,6 +356,8 @@
     <tableColumn id="5" xr3:uid="{2AC59C68-094C-4C75-8924-EACAA4C72BD1}" name="Office"/>
     <tableColumn id="10" xr3:uid="{70A0FA65-7F00-43A2-AA4C-70B8DBDE75A6}" name="City"/>
     <tableColumn id="11" xr3:uid="{285F77D6-2A79-4307-9E56-8B2611B6C5DA}" name="State"/>
+    <tableColumn id="15" xr3:uid="{86DB94BD-715B-42BE-9B24-4B44124B2FD2}" name="SPS-Skills" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{678D10E1-42F1-43B1-9DE2-3AAEBBAA9B16}" name="SPS-School" dataDxfId="0"/>
     <tableColumn id="13" xr3:uid="{53E7A27A-826C-4261-9349-F14D4C12AB2A}" name="Office365Plans"/>
     <tableColumn id="12" xr3:uid="{B514E4A6-C6AC-4889-898A-AA1A53287E36}" name="AccountEnabled"/>
     <tableColumn id="4" xr3:uid="{76BA5797-6ED4-4FAD-AD0D-BDB4873AFC64}" name="UsageLocation"/>
@@ -555,11 +662,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4357D9CC-3F8E-4B3B-B352-13C40438E850}">
+  <dimension ref="B2:C3"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="66.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA39548C-6792-479F-B44E-E97CE90FF367}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,11 +713,15 @@
     <col min="1" max="2" width="22.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="12" width="22.42578125" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" customWidth="1"/>
+    <col min="5" max="10" width="22.42578125" customWidth="1"/>
+    <col min="11" max="11" width="60.85546875" customWidth="1"/>
+    <col min="12" max="12" width="60.85546875" style="6" customWidth="1"/>
+    <col min="13" max="13" width="33.85546875" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -603,16 +753,22 @@
         <v>35</v>
       </c>
       <c r="K1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" t="s">
         <v>37</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>34</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>drstrange</v>
@@ -644,17 +800,24 @@
       <c r="J2" t="s">
         <v>31</v>
       </c>
-      <c r="K2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2" t="b">
+      <c r="K2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" t="str">
+        <f>Office365Plans</f>
+        <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
+      </c>
+      <c r="N2" t="b">
         <v>1</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>drwatt</v>
@@ -686,17 +849,24 @@
       <c r="J3" t="s">
         <v>32</v>
       </c>
-      <c r="K3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" t="b">
+      <c r="K3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" t="str">
+        <f>Office365Plans</f>
+        <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
+      </c>
+      <c r="N3" t="b">
         <v>1</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>nursejazz</v>
@@ -728,17 +898,22 @@
       <c r="J4" t="s">
         <v>32</v>
       </c>
-      <c r="K4" t="s">
-        <v>36</v>
-      </c>
-      <c r="L4" t="b">
+      <c r="K4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="7"/>
+      <c r="M4" t="str">
+        <f>Office365Plans</f>
+        <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
+      </c>
+      <c r="N4" t="b">
         <v>1</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>nursesmith</v>
@@ -770,13 +945,16 @@
       <c r="J5" t="s">
         <v>31</v>
       </c>
-      <c r="K5" t="s">
-        <v>36</v>
-      </c>
-      <c r="L5" t="b">
+      <c r="K5" s="5"/>
+      <c r="L5" s="7"/>
+      <c r="M5" t="str">
+        <f>Office365Plans</f>
+        <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
+      </c>
+      <c r="N5" t="b">
         <v>1</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Manager property now set in Azure AD.
</commit_message>
<xml_diff>
--- a/personas.xlsx
+++ b/personas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\SmartterHealth\content-personas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BEAA16F7-71DC-4514-9E91-97521D0D43F5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{396778B9-E874-4A37-AD41-F5F6B50DD4BB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12990" activeTab="1" xr2:uid="{87C741E5-9606-4A4F-9009-1E4112E4DF41}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>FirstName</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>Shrini</t>
+  </si>
+  <si>
+    <t>Manager</t>
   </si>
 </sst>
 </file>
@@ -309,12 +312,15 @@
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -355,19 +361,20 @@
   <autoFilter ref="B2:C3" xr:uid="{51B885EE-B54A-4B22-8BBE-6A24E37364BA}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{13495667-CD26-47D2-852E-FE8A0243D3F3}" name="Input" dataCellStyle="Good"/>
-    <tableColumn id="2" xr3:uid="{1CA1CBF2-D93F-4341-A6C1-6E4D4F42645E}" name="Value" dataDxfId="3" dataCellStyle="Accent6"/>
+    <tableColumn id="2" xr3:uid="{1CA1CBF2-D93F-4341-A6C1-6E4D4F42645E}" name="Value" dataDxfId="4" dataCellStyle="Accent6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A05BCBD-9362-4444-B6D3-C1287FB470BC}" name="Table1" displayName="Table1" ref="A1:O6" totalsRowShown="0">
-  <autoFilter ref="A1:O6" xr:uid="{F11B011F-1E1B-4583-908A-0C59183AED54}"/>
-  <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{236BF943-7CEB-4C17-8BA7-42A7146DF91F}" name="Alias" dataDxfId="2" dataCellStyle="Calculation">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A05BCBD-9362-4444-B6D3-C1287FB470BC}" name="Table1" displayName="Table1" ref="A1:P6" totalsRowShown="0">
+  <autoFilter ref="A1:P6" xr:uid="{F11B011F-1E1B-4583-908A-0C59183AED54}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{236BF943-7CEB-4C17-8BA7-42A7146DF91F}" name="Alias" dataDxfId="3" dataCellStyle="Calculation">
       <calculatedColumnFormula>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="14" xr3:uid="{933DEACC-F0A2-4CA4-AD1A-FEC4844881AD}" name="Manager" dataDxfId="2" dataCellStyle="Calculation"/>
     <tableColumn id="7" xr3:uid="{6FCDF76C-45C2-4AB8-8CC1-20BA4C805A59}" name="Title"/>
     <tableColumn id="2" xr3:uid="{E62E75CD-5A0E-4B86-AF35-B991CBE33DD8}" name="FirstName"/>
     <tableColumn id="3" xr3:uid="{4B996375-CD17-402D-8BEB-D35A4E982B2E}" name="LastName"/>
@@ -723,303 +730,317 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA39548C-6792-479F-B44E-E97CE90FF367}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="10" width="22.42578125" customWidth="1"/>
-    <col min="11" max="11" width="60.85546875" customWidth="1"/>
-    <col min="12" max="12" width="60.85546875" style="6" customWidth="1"/>
-    <col min="13" max="13" width="33.85546875" customWidth="1"/>
-    <col min="14" max="14" width="22.42578125" customWidth="1"/>
-    <col min="15" max="15" width="17.85546875" customWidth="1"/>
+    <col min="1" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="11" width="22.42578125" customWidth="1"/>
+    <col min="12" max="12" width="60.85546875" customWidth="1"/>
+    <col min="13" max="13" width="60.85546875" style="6" customWidth="1"/>
+    <col min="14" max="14" width="33.85546875" customWidth="1"/>
+    <col min="15" max="15" width="22.42578125" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>37</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>34</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>55</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>54</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>47</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>50</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>27</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>48</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="N2" t="b">
+      <c r="N2" t="str">
+        <f>Office365Plans</f>
+        <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
+      </c>
+      <c r="O2" t="b">
         <v>1</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>drstrange</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>29</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="M3" t="str">
+      <c r="N3" t="str">
         <f>Office365Plans</f>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="N3" t="b">
+      <c r="O3" t="b">
         <v>1</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>drwatt</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>33</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>27</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>30</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="M4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="M4" t="str">
+      <c r="N4" t="str">
         <f>Office365Plans</f>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="N4" t="b">
+      <c r="O4" t="b">
         <v>1</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>nursejazz</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>12</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>33</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>27</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>30</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L5" s="7"/>
-      <c r="M5" t="str">
+      <c r="M5" s="7"/>
+      <c r="N5" t="str">
         <f>Office365Plans</f>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="N5" t="b">
+      <c r="O5" t="b">
         <v>1</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>nursesmith</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>26</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>21</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>23</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>29</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="7"/>
-      <c r="M6" t="str">
+      <c r="L6" s="5"/>
+      <c r="M6" s="7"/>
+      <c r="N6" t="str">
         <f>Office365Plans</f>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="N6" t="b">
+      <c r="O6" t="b">
         <v>1</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Order of user creation corrected
The order of when users are created in relation to their manager is now correct
</commit_message>
<xml_diff>
--- a/personas.xlsx
+++ b/personas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\SmartterHealth\content-personas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{396778B9-E874-4A37-AD41-F5F6B50DD4BB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{ED111460-2848-492D-BD69-447195C6D8E2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12990" activeTab="1" xr2:uid="{87C741E5-9606-4A4F-9009-1E4112E4DF41}"/>
   </bookViews>
@@ -17,7 +17,9 @@
     <sheet name="personas" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Office365Plans">GlobalInputs[Value]</definedName>
+    <definedName name="AccountEnabled">inputs!$C$4</definedName>
+    <definedName name="Office365Plans">inputs!$C$3</definedName>
+    <definedName name="UsageLocation">inputs!$C$5</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="72">
   <si>
     <t>FirstName</t>
   </si>
@@ -79,12 +81,6 @@
     <t>Dr. Strange</t>
   </si>
   <si>
-    <t>Nurse Jazz</t>
-  </si>
-  <si>
-    <t>Dr. Watt</t>
-  </si>
-  <si>
     <t>JobTitle</t>
   </si>
   <si>
@@ -109,9 +105,6 @@
     <t>Smith</t>
   </si>
   <si>
-    <t>Nurse Nancy</t>
-  </si>
-  <si>
     <t>Building 2</t>
   </si>
   <si>
@@ -172,9 +165,6 @@
     <t>Baylor University;John Hopkins University</t>
   </si>
   <si>
-    <t>Dr. Patel</t>
-  </si>
-  <si>
     <t>Minneapolis</t>
   </si>
   <si>
@@ -200,13 +190,70 @@
   </si>
   <si>
     <t>Manager</t>
+  </si>
+  <si>
+    <t>drparsons</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Parsons</t>
+  </si>
+  <si>
+    <t>Dr. Robert Parsons</t>
+  </si>
+  <si>
+    <t>Nurse Holly Jazz</t>
+  </si>
+  <si>
+    <t>Nurse Nancy Smith</t>
+  </si>
+  <si>
+    <t>Dr. Shrini Patel</t>
+  </si>
+  <si>
+    <t>Dr. J.J Watt</t>
+  </si>
+  <si>
+    <t>Building 3</t>
+  </si>
+  <si>
+    <t>drjosh</t>
+  </si>
+  <si>
+    <t>Josh</t>
+  </si>
+  <si>
+    <t>Simmons</t>
+  </si>
+  <si>
+    <t>D. Josh Simmons</t>
+  </si>
+  <si>
+    <t>OrgLevel</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Separate mutiple values with a semi-colon.</t>
+  </si>
+  <si>
+    <t>Account Enabled</t>
+  </si>
+  <si>
+    <t>Office 365 Plans</t>
+  </si>
+  <si>
+    <t>Usage Location</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +283,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -260,7 +315,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -283,6 +338,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -290,12 +367,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -305,6 +381,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent6" xfId="3" builtinId="49"/>
@@ -312,7 +405,45 @@
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="2" tint="-0.89996032593768116"/>
+        </left>
+        <right style="thin">
+          <color theme="2" tint="-0.89996032593768116"/>
+        </right>
+        <top style="thin">
+          <color theme="2" tint="-0.89996032593768116"/>
+        </top>
+        <bottom style="thin">
+          <color theme="2" tint="-0.89996032593768116"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -326,7 +457,11 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF7F7F7F"/>
         </left>
@@ -339,8 +474,13 @@
         <bottom style="thin">
           <color rgb="FF7F7F7F"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color rgb="FF7F7F7F"/>
+        </right>
       </border>
     </dxf>
   </dxfs>
@@ -357,24 +497,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EE6B63CB-DF51-44B2-B6E1-268D302375BC}" name="GlobalInputs" displayName="GlobalInputs" ref="B2:C3" totalsRowShown="0">
-  <autoFilter ref="B2:C3" xr:uid="{51B885EE-B54A-4B22-8BBE-6A24E37364BA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EE6B63CB-DF51-44B2-B6E1-268D302375BC}" name="GlobalInputs" displayName="GlobalInputs" ref="B2:C5" totalsRowShown="0">
+  <autoFilter ref="B2:C5" xr:uid="{51B885EE-B54A-4B22-8BBE-6A24E37364BA}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{13495667-CD26-47D2-852E-FE8A0243D3F3}" name="Input" dataCellStyle="Good"/>
-    <tableColumn id="2" xr3:uid="{1CA1CBF2-D93F-4341-A6C1-6E4D4F42645E}" name="Value" dataDxfId="4" dataCellStyle="Accent6"/>
+    <tableColumn id="1" xr3:uid="{13495667-CD26-47D2-852E-FE8A0243D3F3}" name="Input" dataDxfId="8" dataCellStyle="Good"/>
+    <tableColumn id="2" xr3:uid="{1CA1CBF2-D93F-4341-A6C1-6E4D4F42645E}" name="Value" dataDxfId="7" dataCellStyle="Accent6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A05BCBD-9362-4444-B6D3-C1287FB470BC}" name="Table1" displayName="Table1" ref="A1:P6" totalsRowShown="0">
-  <autoFilter ref="A1:P6" xr:uid="{F11B011F-1E1B-4583-908A-0C59183AED54}"/>
-  <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{236BF943-7CEB-4C17-8BA7-42A7146DF91F}" name="Alias" dataDxfId="3" dataCellStyle="Calculation">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A05BCBD-9362-4444-B6D3-C1287FB470BC}" name="Table1" displayName="Table1" ref="A1:Q8" totalsRowShown="0">
+  <autoFilter ref="A1:Q8" xr:uid="{F11B011F-1E1B-4583-908A-0C59183AED54}"/>
+  <sortState ref="B2:Q7">
+    <sortCondition descending="1" ref="C1:C7"/>
+  </sortState>
+  <tableColumns count="17">
+    <tableColumn id="17" xr3:uid="{51014DA3-E404-4390-9CD9-9EB23597CC53}" name="OrgLevel" dataDxfId="6" dataCellStyle="Calculation"/>
+    <tableColumn id="1" xr3:uid="{236BF943-7CEB-4C17-8BA7-42A7146DF91F}" name="Alias" dataDxfId="5" dataCellStyle="Calculation">
       <calculatedColumnFormula>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{933DEACC-F0A2-4CA4-AD1A-FEC4844881AD}" name="Manager" dataDxfId="2" dataCellStyle="Calculation"/>
+    <tableColumn id="14" xr3:uid="{933DEACC-F0A2-4CA4-AD1A-FEC4844881AD}" name="Manager" dataDxfId="4" dataCellStyle="Calculation"/>
     <tableColumn id="7" xr3:uid="{6FCDF76C-45C2-4AB8-8CC1-20BA4C805A59}" name="Title"/>
     <tableColumn id="2" xr3:uid="{E62E75CD-5A0E-4B86-AF35-B991CBE33DD8}" name="FirstName"/>
     <tableColumn id="3" xr3:uid="{4B996375-CD17-402D-8BEB-D35A4E982B2E}" name="LastName"/>
@@ -384,9 +528,11 @@
     <tableColumn id="5" xr3:uid="{2AC59C68-094C-4C75-8924-EACAA4C72BD1}" name="Office"/>
     <tableColumn id="10" xr3:uid="{70A0FA65-7F00-43A2-AA4C-70B8DBDE75A6}" name="City"/>
     <tableColumn id="11" xr3:uid="{285F77D6-2A79-4307-9E56-8B2611B6C5DA}" name="State"/>
-    <tableColumn id="15" xr3:uid="{86DB94BD-715B-42BE-9B24-4B44124B2FD2}" name="SPS-Skills" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{678D10E1-42F1-43B1-9DE2-3AAEBBAA9B16}" name="SPS-School" dataDxfId="0"/>
-    <tableColumn id="13" xr3:uid="{53E7A27A-826C-4261-9349-F14D4C12AB2A}" name="Office365Plans"/>
+    <tableColumn id="15" xr3:uid="{86DB94BD-715B-42BE-9B24-4B44124B2FD2}" name="SPS-Skills" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{678D10E1-42F1-43B1-9DE2-3AAEBBAA9B16}" name="SPS-School" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{53E7A27A-826C-4261-9349-F14D4C12AB2A}" name="Office365Plans">
+      <calculatedColumnFormula>Office365Plans</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="12" xr3:uid="{B514E4A6-C6AC-4889-898A-AA1A53287E36}" name="AccountEnabled"/>
     <tableColumn id="4" xr3:uid="{76BA5797-6ED4-4FAD-AD0D-BDB4873AFC64}" name="UsageLocation"/>
   </tableColumns>
@@ -691,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4357D9CC-3F8E-4B3B-B352-13C40438E850}">
-  <dimension ref="B2:C3"/>
+  <dimension ref="B1:C5"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,20 +849,41 @@
     <col min="3" max="3" width="66.42578125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>36</v>
+        <v>70</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -730,321 +897,462 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA39548C-6792-479F-B44E-E97CE90FF367}">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="11" width="22.42578125" customWidth="1"/>
     <col min="12" max="12" width="60.85546875" customWidth="1"/>
-    <col min="13" max="13" width="60.85546875" style="6" customWidth="1"/>
+    <col min="13" max="13" width="60.85546875" style="5" customWidth="1"/>
     <col min="14" max="14" width="33.85546875" customWidth="1"/>
     <col min="15" max="15" width="22.42578125" customWidth="1"/>
     <col min="16" max="16" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>56</v>
-      </c>
       <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" t="s">
-        <v>28</v>
-      </c>
       <c r="K1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="N1" t="s">
-        <v>37</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
       </c>
       <c r="P1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
+        <v>drwatt</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" t="str">
+        <f t="shared" ref="O2:O8" si="0">Office365Plans</f>
+        <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
+      </c>
+      <c r="P2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="str">
+        <f t="shared" ref="Q2:Q8" si="1">UsageLocation</f>
+        <v>US</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" t="s">
+      <c r="C3" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="9"/>
+      <c r="N3" s="10"/>
+      <c r="O3" t="str">
+        <f t="shared" si="0"/>
+        <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
+      </c>
+      <c r="P3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="str">
+        <f t="shared" si="1"/>
+        <v>US</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="N4" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2" t="str">
-        <f>Office365Plans</f>
+      <c r="O4" t="str">
+        <f t="shared" si="0"/>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="O2" t="b">
+      <c r="P4" t="b">
         <v>1</v>
       </c>
-      <c r="P2" t="s">
-        <v>6</v>
+      <c r="Q4" t="str">
+        <f t="shared" si="1"/>
+        <v>US</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="str">
+    <row r="5" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>drstrange</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F5" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G5" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J5" t="s">
         <v>21</v>
       </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="5" t="s">
+      <c r="K5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="N3" t="str">
-        <f>Office365Plans</f>
+      <c r="O5" t="str">
+        <f t="shared" si="0"/>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="O3" t="b">
+      <c r="P5" t="b">
         <v>1</v>
       </c>
-      <c r="P3" t="s">
-        <v>6</v>
+      <c r="Q5" t="str">
+        <f t="shared" si="1"/>
+        <v>US</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="str">
-        <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
-        <v>drwatt</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="N4" t="str">
-        <f>Office365Plans</f>
-        <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
-      </c>
-      <c r="O4" t="b">
-        <v>1</v>
-      </c>
-      <c r="P4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="str">
+    <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>nursejazz</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F6" t="s">
         <v>14</v>
       </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="G6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" t="s">
         <v>12</v>
       </c>
-      <c r="H5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="I6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" t="s">
         <v>27</v>
       </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="M5" s="7"/>
-      <c r="N5" t="str">
-        <f>Office365Plans</f>
+      <c r="L6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="0"/>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="O5" t="b">
+      <c r="P6" t="b">
         <v>1</v>
       </c>
-      <c r="P5" t="s">
-        <v>6</v>
+      <c r="Q6" t="str">
+        <f t="shared" si="1"/>
+        <v>US</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="str">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>nursesmith</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" t="s">
+      <c r="C7" s="7"/>
+      <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" t="s">
         <v>26</v>
       </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="7"/>
-      <c r="N6" t="str">
-        <f>Office365Plans</f>
+      <c r="L7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="0"/>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="O6" t="b">
+      <c r="P7" t="b">
         <v>1</v>
       </c>
-      <c r="P6" t="s">
-        <v>6</v>
+      <c r="Q7" t="str">
+        <f t="shared" si="1"/>
+        <v>US</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>3</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="0"/>
+        <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
+      </c>
+      <c r="P8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="1"/>
+        <v>US</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:Q1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
#Issue #2 - User  manager is not properly set.
</commit_message>
<xml_diff>
--- a/personas.xlsx
+++ b/personas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\SmartterHealth\content-personas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{ED111460-2848-492D-BD69-447195C6D8E2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8053DE37-BCF8-4CAB-8890-6C422ACF28AB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12990" activeTab="1" xr2:uid="{87C741E5-9606-4A4F-9009-1E4112E4DF41}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
   <si>
     <t>FirstName</t>
   </si>
@@ -228,12 +228,6 @@
     <t>Simmons</t>
   </si>
   <si>
-    <t>D. Josh Simmons</t>
-  </si>
-  <si>
-    <t>OrgLevel</t>
-  </si>
-  <si>
     <t>TBD</t>
   </si>
   <si>
@@ -247,6 +241,9 @@
   </si>
   <si>
     <t>Usage Location</t>
+  </si>
+  <si>
+    <t>Dr. Josh Simmons</t>
   </si>
 </sst>
 </file>
@@ -405,18 +402,7 @@
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <b/>
@@ -449,9 +435,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -500,25 +483,24 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EE6B63CB-DF51-44B2-B6E1-268D302375BC}" name="GlobalInputs" displayName="GlobalInputs" ref="B2:C5" totalsRowShown="0">
   <autoFilter ref="B2:C5" xr:uid="{51B885EE-B54A-4B22-8BBE-6A24E37364BA}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{13495667-CD26-47D2-852E-FE8A0243D3F3}" name="Input" dataDxfId="8" dataCellStyle="Good"/>
-    <tableColumn id="2" xr3:uid="{1CA1CBF2-D93F-4341-A6C1-6E4D4F42645E}" name="Value" dataDxfId="7" dataCellStyle="Accent6"/>
+    <tableColumn id="1" xr3:uid="{13495667-CD26-47D2-852E-FE8A0243D3F3}" name="Input" dataDxfId="6" dataCellStyle="Good"/>
+    <tableColumn id="2" xr3:uid="{1CA1CBF2-D93F-4341-A6C1-6E4D4F42645E}" name="Value" dataDxfId="5" dataCellStyle="Accent6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A05BCBD-9362-4444-B6D3-C1287FB470BC}" name="Table1" displayName="Table1" ref="A1:Q8" totalsRowShown="0">
-  <autoFilter ref="A1:Q8" xr:uid="{F11B011F-1E1B-4583-908A-0C59183AED54}"/>
-  <sortState ref="B2:Q7">
-    <sortCondition descending="1" ref="C1:C7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A05BCBD-9362-4444-B6D3-C1287FB470BC}" name="Table1" displayName="Table1" ref="A1:P8" totalsRowShown="0">
+  <autoFilter ref="A1:P8" xr:uid="{F11B011F-1E1B-4583-908A-0C59183AED54}"/>
+  <sortState ref="A2:P7">
+    <sortCondition descending="1" ref="B1:B7"/>
   </sortState>
-  <tableColumns count="17">
-    <tableColumn id="17" xr3:uid="{51014DA3-E404-4390-9CD9-9EB23597CC53}" name="OrgLevel" dataDxfId="6" dataCellStyle="Calculation"/>
-    <tableColumn id="1" xr3:uid="{236BF943-7CEB-4C17-8BA7-42A7146DF91F}" name="Alias" dataDxfId="5" dataCellStyle="Calculation">
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{236BF943-7CEB-4C17-8BA7-42A7146DF91F}" name="Alias" dataDxfId="4" dataCellStyle="Calculation">
       <calculatedColumnFormula>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{933DEACC-F0A2-4CA4-AD1A-FEC4844881AD}" name="Manager" dataDxfId="4" dataCellStyle="Calculation"/>
+    <tableColumn id="14" xr3:uid="{933DEACC-F0A2-4CA4-AD1A-FEC4844881AD}" name="Manager" dataDxfId="3" dataCellStyle="Calculation"/>
     <tableColumn id="7" xr3:uid="{6FCDF76C-45C2-4AB8-8CC1-20BA4C805A59}" name="Title"/>
     <tableColumn id="2" xr3:uid="{E62E75CD-5A0E-4B86-AF35-B991CBE33DD8}" name="FirstName"/>
     <tableColumn id="3" xr3:uid="{4B996375-CD17-402D-8BEB-D35A4E982B2E}" name="LastName"/>
@@ -528,8 +510,8 @@
     <tableColumn id="5" xr3:uid="{2AC59C68-094C-4C75-8924-EACAA4C72BD1}" name="Office"/>
     <tableColumn id="10" xr3:uid="{70A0FA65-7F00-43A2-AA4C-70B8DBDE75A6}" name="City"/>
     <tableColumn id="11" xr3:uid="{285F77D6-2A79-4307-9E56-8B2611B6C5DA}" name="State"/>
-    <tableColumn id="15" xr3:uid="{86DB94BD-715B-42BE-9B24-4B44124B2FD2}" name="SPS-Skills" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{678D10E1-42F1-43B1-9DE2-3AAEBBAA9B16}" name="SPS-School" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{86DB94BD-715B-42BE-9B24-4B44124B2FD2}" name="SPS-Skills" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{678D10E1-42F1-43B1-9DE2-3AAEBBAA9B16}" name="SPS-School" dataDxfId="1"/>
     <tableColumn id="13" xr3:uid="{53E7A27A-826C-4261-9349-F14D4C12AB2A}" name="Office365Plans">
       <calculatedColumnFormula>Office365Plans</calculatedColumnFormula>
     </tableColumn>
@@ -851,7 +833,7 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C1" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
@@ -864,7 +846,7 @@
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>33</v>
@@ -872,7 +854,7 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C4" s="13" t="b">
         <v>1</v>
@@ -880,7 +862,7 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>6</v>
@@ -897,459 +879,434 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA39548C-6792-479F-B44E-E97CE90FF367}">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="11" width="22.42578125" customWidth="1"/>
-    <col min="12" max="12" width="60.85546875" customWidth="1"/>
-    <col min="13" max="13" width="60.85546875" style="5" customWidth="1"/>
-    <col min="14" max="14" width="33.85546875" customWidth="1"/>
-    <col min="15" max="15" width="22.42578125" customWidth="1"/>
-    <col min="16" max="16" width="17.85546875" customWidth="1"/>
+    <col min="1" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="10" width="22.42578125" customWidth="1"/>
+    <col min="11" max="11" width="60.85546875" customWidth="1"/>
+    <col min="12" max="12" width="60.85546875" style="5" customWidth="1"/>
+    <col min="13" max="13" width="33.85546875" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="H1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="L1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>40</v>
       </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
       <c r="O1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="P1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="str">
+    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>drwatt</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" t="str">
+        <f t="shared" ref="N2:N8" si="0">Office365Plans</f>
+        <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
+      </c>
+      <c r="O2" t="b">
+        <v>1</v>
+      </c>
+      <c r="P2" t="str">
+        <f t="shared" ref="P2:P8" si="1">UsageLocation</f>
+        <v>US</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="D3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="H3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="O2" t="str">
-        <f t="shared" ref="O2:O8" si="0">Office365Plans</f>
-        <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
-      </c>
-      <c r="P2" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="str">
-        <f t="shared" ref="Q2:Q8" si="1">UsageLocation</f>
-        <v>US</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="J3" s="8" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="L3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="M3" s="9"/>
-      <c r="N3" s="10"/>
-      <c r="O3" t="str">
+      <c r="L3" s="9"/>
+      <c r="M3" s="10"/>
+      <c r="N3" t="str">
         <f t="shared" si="0"/>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="P3" t="b">
+      <c r="O3" t="b">
         <v>1</v>
       </c>
-      <c r="Q3" t="str">
+      <c r="P3" t="str">
         <f t="shared" si="1"/>
         <v>US</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="I4" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="K4" t="s">
-        <v>44</v>
-      </c>
-      <c r="L4" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="M4" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="O4" t="str">
+      <c r="N4" t="str">
         <f t="shared" si="0"/>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="P4" t="b">
+      <c r="O4" t="b">
         <v>1</v>
       </c>
-      <c r="Q4" t="str">
+      <c r="P4" t="str">
         <f t="shared" si="1"/>
         <v>US</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="str">
+    <row r="5" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>drstrange</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="M5" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="O5" t="str">
+      <c r="N5" t="str">
         <f t="shared" si="0"/>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="P5" t="b">
+      <c r="O5" t="b">
         <v>1</v>
       </c>
-      <c r="Q5" t="str">
+      <c r="P5" t="str">
         <f t="shared" si="1"/>
         <v>US</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2" t="str">
+    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>nursejazz</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
       <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>57</v>
-      </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="I6" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="J6" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="K6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L6" t="s">
         <v>29</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="L6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N6" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="O6" t="str">
+      <c r="M6" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="N6" t="str">
         <f t="shared" si="0"/>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="P6" t="b">
+      <c r="O6" t="b">
         <v>1</v>
       </c>
-      <c r="Q6" t="str">
+      <c r="P6" t="str">
         <f t="shared" si="1"/>
         <v>US</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>2</v>
-      </c>
-      <c r="B7" s="7" t="str">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>nursesmith</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
       <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" t="s">
-        <v>58</v>
-      </c>
       <c r="H7" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="K7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" t="s">
         <v>28</v>
       </c>
-      <c r="M7" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="O7" t="str">
+      <c r="L7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="N7" t="str">
         <f t="shared" si="0"/>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="P7" t="b">
+      <c r="O7" t="b">
         <v>1</v>
       </c>
-      <c r="Q7" t="str">
+      <c r="P7" t="str">
         <f t="shared" si="1"/>
         <v>US</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>3</v>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="7" t="s">
         <v>53</v>
       </c>
+      <c r="C8" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="D8" s="8" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="G8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="H8" s="8" t="s">
-        <v>17</v>
-      </c>
       <c r="I8" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="O8" t="str">
+        <v>65</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="N8" t="str">
         <f t="shared" si="0"/>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="P8" t="b">
+      <c r="O8" t="b">
         <v>1</v>
       </c>
-      <c r="Q8" t="str">
+      <c r="P8" t="str">
         <f t="shared" si="1"/>
         <v>US</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:Q1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="A1:P1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
SharePoint skills and schools now working.
</commit_message>
<xml_diff>
--- a/personas.xlsx
+++ b/personas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\SmartterHealth\content-personas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8053DE37-BCF8-4CAB-8890-6C422ACF28AB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFF606B7-66CE-418B-8E9A-D9F769A82981}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12990" activeTab="1" xr2:uid="{87C741E5-9606-4A4F-9009-1E4112E4DF41}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
   <si>
     <t>FirstName</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Jazz</t>
   </si>
   <si>
-    <t>Dr. Strange</t>
-  </si>
-  <si>
     <t>JobTitle</t>
   </si>
   <si>
@@ -144,18 +141,12 @@
     <t>Input</t>
   </si>
   <si>
-    <t>SPS-Skills</t>
-  </si>
-  <si>
     <t>Hospital Medicine;Hospital Management;Outcomes Research;Teaching;Strategic Planning;EMR;Innovation</t>
   </si>
   <si>
     <t>Cardiopulmonary Physical Therapy;Heat Illness Prevention;CITI Program - Human Subject Research</t>
   </si>
   <si>
-    <t>SPS-School</t>
-  </si>
-  <si>
     <t>Vanderbilt University School of Medicine;University of Tennessee - Knoxville</t>
   </si>
   <si>
@@ -201,21 +192,6 @@
     <t>Parsons</t>
   </si>
   <si>
-    <t>Dr. Robert Parsons</t>
-  </si>
-  <si>
-    <t>Nurse Holly Jazz</t>
-  </si>
-  <si>
-    <t>Nurse Nancy Smith</t>
-  </si>
-  <si>
-    <t>Dr. Shrini Patel</t>
-  </si>
-  <si>
-    <t>Dr. J.J Watt</t>
-  </si>
-  <si>
     <t>Building 3</t>
   </si>
   <si>
@@ -243,14 +219,17 @@
     <t>Usage Location</t>
   </si>
   <si>
-    <t>Dr. Josh Simmons</t>
+    <t>Skills</t>
+  </si>
+  <si>
+    <t>School</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,8 +267,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -311,8 +298,13 @@
         <fgColor theme="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -357,14 +349,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
@@ -395,10 +403,12 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Accent6" xfId="3" builtinId="49"/>
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -504,14 +514,14 @@
     <tableColumn id="7" xr3:uid="{6FCDF76C-45C2-4AB8-8CC1-20BA4C805A59}" name="Title"/>
     <tableColumn id="2" xr3:uid="{E62E75CD-5A0E-4B86-AF35-B991CBE33DD8}" name="FirstName"/>
     <tableColumn id="3" xr3:uid="{4B996375-CD17-402D-8BEB-D35A4E982B2E}" name="LastName"/>
-    <tableColumn id="6" xr3:uid="{4261D67B-BCA8-4DC2-BA94-7E9D8E51AEDD}" name="DisplayName"/>
+    <tableColumn id="6" xr3:uid="{4261D67B-BCA8-4DC2-BA94-7E9D8E51AEDD}" name="DisplayName" dataCellStyle="Check Cell"/>
     <tableColumn id="8" xr3:uid="{9A0DF3BC-30FC-4022-B66D-3D4FEF34CCF1}" name="JobTitle"/>
     <tableColumn id="9" xr3:uid="{0454B832-5924-4E24-92DC-9D0F8248A5C2}" name="Department"/>
     <tableColumn id="5" xr3:uid="{2AC59C68-094C-4C75-8924-EACAA4C72BD1}" name="Office"/>
     <tableColumn id="10" xr3:uid="{70A0FA65-7F00-43A2-AA4C-70B8DBDE75A6}" name="City"/>
     <tableColumn id="11" xr3:uid="{285F77D6-2A79-4307-9E56-8B2611B6C5DA}" name="State"/>
-    <tableColumn id="15" xr3:uid="{86DB94BD-715B-42BE-9B24-4B44124B2FD2}" name="SPS-Skills" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{678D10E1-42F1-43B1-9DE2-3AAEBBAA9B16}" name="SPS-School" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{86DB94BD-715B-42BE-9B24-4B44124B2FD2}" name="Skills" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{678D10E1-42F1-43B1-9DE2-3AAEBBAA9B16}" name="School" dataDxfId="1"/>
     <tableColumn id="13" xr3:uid="{53E7A27A-826C-4261-9349-F14D4C12AB2A}" name="Office365Plans">
       <calculatedColumnFormula>Office365Plans</calculatedColumnFormula>
     </tableColumn>
@@ -833,28 +843,28 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C1" s="12" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C4" s="13" t="b">
         <v>1</v>
@@ -862,7 +872,7 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>6</v>
@@ -879,10 +889,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA39548C-6792-479F-B44E-E97CE90FF367}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,12 +908,12 @@
     <col min="15" max="15" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -918,43 +928,43 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L1" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="N1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>drwatt</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -965,29 +975,30 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
-        <v>60</v>
+      <c r="F2" s="16" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[Title]], " ", Table1[[#This Row],[FirstName]], " ", Table1[[#This Row],[LastName]])</f>
+        <v>Dr. J.J. Watt</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="N2" t="str">
         <f t="shared" ref="N2:N8" si="0">Office365Plans</f>
@@ -1001,39 +1012,40 @@
         <v>US</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
+      </c>
+      <c r="F3" s="16" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[Title]], " ", Table1[[#This Row],[FirstName]], " ", Table1[[#This Row],[LastName]])</f>
+        <v>Dr. Robert Parsons</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L3" s="9"/>
       <c r="M3" s="10"/>
@@ -1049,43 +1061,44 @@
         <v>US</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" t="s">
-        <v>59</v>
+        <v>47</v>
+      </c>
+      <c r="F4" s="16" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[Title]], " ", Table1[[#This Row],[FirstName]], " ", Table1[[#This Row],[LastName]])</f>
+        <v>Dr. Shrini Patel</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="N4" t="str">
         <f t="shared" si="0"/>
@@ -1099,7 +1112,7 @@
         <v>US</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>drstrange</v>
@@ -1114,29 +1127,30 @@
       <c r="E5" t="s">
         <v>5</v>
       </c>
-      <c r="F5" t="s">
-        <v>15</v>
+      <c r="F5" s="16" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[Title]], " ", Table1[[#This Row],[FirstName]], " ", Table1[[#This Row],[LastName]])</f>
+        <v>Dr. Stephen Strange</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>41</v>
       </c>
       <c r="N5" t="str">
         <f t="shared" si="0"/>
@@ -1150,7 +1164,7 @@
         <v>US</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>nursejazz</v>
@@ -1165,29 +1179,30 @@
       <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" t="s">
-        <v>57</v>
+      <c r="F6" s="16" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[Title]], " ", Table1[[#This Row],[FirstName]], " ", Table1[[#This Row],[LastName]])</f>
+        <v>Nurse Holly Jazz</v>
       </c>
       <c r="G6" t="s">
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I6" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="J6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" si="0"/>
@@ -1201,7 +1216,7 @@
         <v>US</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>nursesmith</v>
@@ -1211,34 +1226,35 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" t="s">
-        <v>58</v>
+      <c r="F7" s="16" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[Title]], " ", Table1[[#This Row],[FirstName]], " ", Table1[[#This Row],[LastName]])</f>
+        <v>Nurse Nancy Smith</v>
       </c>
       <c r="G7" t="s">
         <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="N7" t="str">
         <f t="shared" si="0"/>
@@ -1252,45 +1268,46 @@
         <v>US</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>70</v>
+        <v>56</v>
+      </c>
+      <c r="F8" s="16" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[Title]], " ", Table1[[#This Row],[FirstName]], " ", Table1[[#This Row],[LastName]])</f>
+        <v>Dr. Josh Simmons</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" si="0"/>
@@ -1304,6 +1321,7 @@
         <v>US</v>
       </c>
     </row>
+    <row r="9" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A1:P1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">

</xml_diff>

<commit_message>
Renamed photo for Nurse Smith
It was causing a "file not found" error.
</commit_message>
<xml_diff>
--- a/personas.xlsx
+++ b/personas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\SmartterHealth\content-personas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FE0A3D0C-3751-47BE-8ED2-C46B46096026}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{852A3230-8C43-4417-BA59-F5C7D6773F3B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12990" activeTab="1" xr2:uid="{87C741E5-9606-4A4F-9009-1E4112E4DF41}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="88">
   <si>
     <t>FirstName</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Hospital Medicine;Hospital Management;Outcomes Research;Teaching;Strategic Planning;EMR;Innovation</t>
   </si>
   <si>
-    <t>Cardiopulmonary Physical Therapy;Heat Illness Prevention;CITI Program - Human Subject Research</t>
-  </si>
-  <si>
     <t>Vanderbilt University School of Medicine;University of Tennessee - Knoxville</t>
   </si>
   <si>
@@ -265,6 +262,39 @@
   </si>
   <si>
     <t>Separate mutiple values (Skills, Interests, etc.) with a semi-colon.</t>
+  </si>
+  <si>
+    <t>AboutMe</t>
+  </si>
+  <si>
+    <t>Bring to the table health care strategies to ensure proactive domination. At the end of the day, going forward, a new normal that has evolved from generation X is on the runway heading towards a streamlined cloud solution. User generated content in real-time will have multiple touchpoints for offshoring.</t>
+  </si>
+  <si>
+    <t>Collaboratively administrate empowered markets via plug-and-play networks. Dynamically procrastinate B2C users after installed base benefits. Dramatically visualize customer directed convergence without revolutionary ROI.</t>
+  </si>
+  <si>
+    <t>Stress Management; Ethics; Attention to Detail</t>
+  </si>
+  <si>
+    <t>Cardiopulmonary Physical Therapy;Heat Illness Prevention;CITI Program - Human Subject Research;Stress Management</t>
+  </si>
+  <si>
+    <t>St. David's School of Nursing</t>
+  </si>
+  <si>
+    <t>Vanderbilt University School of Nursing</t>
+  </si>
+  <si>
+    <t>University of Minnesota; Baylor Collecge of Medicine</t>
+  </si>
+  <si>
+    <t>Nursing; Stress Management</t>
+  </si>
+  <si>
+    <t>Health Care Ethics</t>
+  </si>
+  <si>
+    <t>Cancer Treatments</t>
   </si>
 </sst>
 </file>
@@ -485,7 +515,40 @@
     <cellStyle name="Input" xfId="5" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="2" tint="-0.89996032593768116"/>
+        </left>
+        <right style="thin">
+          <color theme="2" tint="-0.89996032593768116"/>
+        </right>
+        <top style="thin">
+          <color theme="2" tint="-0.89996032593768116"/>
+        </top>
+        <bottom style="thin">
+          <color theme="2" tint="-0.89996032593768116"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -521,9 +584,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -572,24 +632,24 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EE6B63CB-DF51-44B2-B6E1-268D302375BC}" name="GlobalInputs" displayName="GlobalInputs" ref="B2:C5" totalsRowShown="0">
   <autoFilter ref="B2:C5" xr:uid="{51B885EE-B54A-4B22-8BBE-6A24E37364BA}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{13495667-CD26-47D2-852E-FE8A0243D3F3}" name="Input" dataDxfId="8" dataCellStyle="Good"/>
-    <tableColumn id="2" xr3:uid="{1CA1CBF2-D93F-4341-A6C1-6E4D4F42645E}" name="Value" dataDxfId="7" dataCellStyle="Accent6"/>
+    <tableColumn id="1" xr3:uid="{13495667-CD26-47D2-852E-FE8A0243D3F3}" name="Input" dataDxfId="10" dataCellStyle="Good"/>
+    <tableColumn id="2" xr3:uid="{1CA1CBF2-D93F-4341-A6C1-6E4D4F42645E}" name="Value" dataDxfId="9" dataCellStyle="Accent6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A05BCBD-9362-4444-B6D3-C1287FB470BC}" name="Table1" displayName="Table1" ref="A1:R8" totalsRowShown="0">
-  <autoFilter ref="A1:R8" xr:uid="{F11B011F-1E1B-4583-908A-0C59183AED54}"/>
-  <sortState ref="A2:R7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A05BCBD-9362-4444-B6D3-C1287FB470BC}" name="Table1" displayName="Table1" ref="A1:S8" totalsRowShown="0">
+  <autoFilter ref="A1:S8" xr:uid="{F11B011F-1E1B-4583-908A-0C59183AED54}"/>
+  <sortState ref="A2:S7">
     <sortCondition descending="1" ref="B1:B7"/>
   </sortState>
-  <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{236BF943-7CEB-4C17-8BA7-42A7146DF91F}" name="Alias" dataDxfId="6" dataCellStyle="Calculation">
+  <tableColumns count="19">
+    <tableColumn id="1" xr3:uid="{236BF943-7CEB-4C17-8BA7-42A7146DF91F}" name="Alias" dataDxfId="8" dataCellStyle="Calculation">
       <calculatedColumnFormula>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{933DEACC-F0A2-4CA4-AD1A-FEC4844881AD}" name="Manager" dataDxfId="5" dataCellStyle="Calculation"/>
+    <tableColumn id="14" xr3:uid="{933DEACC-F0A2-4CA4-AD1A-FEC4844881AD}" name="Manager" dataDxfId="7" dataCellStyle="Calculation"/>
     <tableColumn id="7" xr3:uid="{6FCDF76C-45C2-4AB8-8CC1-20BA4C805A59}" name="Title"/>
     <tableColumn id="2" xr3:uid="{E62E75CD-5A0E-4B86-AF35-B991CBE33DD8}" name="FirstName"/>
     <tableColumn id="3" xr3:uid="{4B996375-CD17-402D-8BEB-D35A4E982B2E}" name="LastName"/>
@@ -599,10 +659,11 @@
     <tableColumn id="5" xr3:uid="{2AC59C68-094C-4C75-8924-EACAA4C72BD1}" name="Office"/>
     <tableColumn id="10" xr3:uid="{70A0FA65-7F00-43A2-AA4C-70B8DBDE75A6}" name="City"/>
     <tableColumn id="11" xr3:uid="{285F77D6-2A79-4307-9E56-8B2611B6C5DA}" name="State"/>
-    <tableColumn id="15" xr3:uid="{86DB94BD-715B-42BE-9B24-4B44124B2FD2}" name="Skills" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{678D10E1-42F1-43B1-9DE2-3AAEBBAA9B16}" name="School" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{0CEE77BE-14D1-462D-A3A2-9198FB58F544}" name="AskMeAbout" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{79E0C1B8-72D0-4920-9AE5-7431EAD192DC}" name="Interests" dataDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{E1889FF8-366D-47D7-BDB9-E1120AE2438F}" name="AboutMe" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{86DB94BD-715B-42BE-9B24-4B44124B2FD2}" name="Skills" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{678D10E1-42F1-43B1-9DE2-3AAEBBAA9B16}" name="School" dataDxfId="6"/>
+    <tableColumn id="17" xr3:uid="{0CEE77BE-14D1-462D-A3A2-9198FB58F544}" name="AskMeAbout" dataDxfId="5"/>
+    <tableColumn id="18" xr3:uid="{79E0C1B8-72D0-4920-9AE5-7431EAD192DC}" name="Interests" dataDxfId="4"/>
     <tableColumn id="13" xr3:uid="{53E7A27A-826C-4261-9349-F14D4C12AB2A}" name="Office365Plans">
       <calculatedColumnFormula>Office365Plans</calculatedColumnFormula>
     </tableColumn>
@@ -932,7 +993,7 @@
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>32</v>
@@ -940,7 +1001,7 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="12" t="b">
         <v>1</v>
@@ -948,7 +1009,7 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>6</v>
@@ -960,23 +1021,23 @@
     </row>
     <row r="7" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>76</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -990,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA39548C-6792-479F-B44E-E97CE90FF367}">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,18 +1070,19 @@
     <col min="9" max="9" width="12" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" customWidth="1"/>
     <col min="11" max="11" width="8.140625" customWidth="1"/>
-    <col min="12" max="12" width="60.85546875" style="5" customWidth="1"/>
-    <col min="13" max="15" width="33.85546875" customWidth="1"/>
-    <col min="16" max="16" width="22.42578125" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" customWidth="1"/>
+    <col min="12" max="12" width="42.5703125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="60.85546875" style="5" customWidth="1"/>
+    <col min="14" max="16" width="33.85546875" customWidth="1"/>
+    <col min="17" max="17" width="22.42578125" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -1049,35 +1111,38 @@
       <c r="K1" t="s">
         <v>31</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="P1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q1" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>30</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>drwatt</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -1108,42 +1173,47 @@
         <v>28</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="N2" s="6"/>
       <c r="O2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="P2" t="str">
-        <f t="shared" ref="P2:P8" si="0">Office365Plans</f>
+        <v>87</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q2" t="str">
+        <f t="shared" ref="Q2:Q8" si="0">Office365Plans</f>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="Q2" t="b">
+      <c r="R2" t="b">
         <v>1</v>
       </c>
-      <c r="R2" t="str">
-        <f t="shared" ref="R2:R8" si="1">UsageLocation</f>
+      <c r="S2" t="str">
+        <f t="shared" ref="S2:S8" si="1">UsageLocation</f>
         <v>US</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>52</v>
       </c>
       <c r="F3" s="15" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Title]], " ", Table1[[#This Row],[FirstName]], " ", Table1[[#This Row],[LastName]])</f>
@@ -1153,48 +1223,57 @@
         <v>16</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>23</v>
       </c>
       <c r="J3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
+      <c r="L3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="O3" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="P3" t="str">
+        <v>87</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q3" t="str">
         <f t="shared" si="0"/>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="Q3" t="b">
+      <c r="R3" t="b">
         <v>1</v>
       </c>
-      <c r="R3" t="str">
+      <c r="S3" t="str">
         <f t="shared" si="1"/>
         <v>US</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F4" s="15" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Title]], " ", Table1[[#This Row],[FirstName]], " ", Table1[[#This Row],[LastName]])</f>
@@ -1204,40 +1283,45 @@
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I4" t="s">
         <v>23</v>
       </c>
       <c r="J4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
         <v>41</v>
       </c>
-      <c r="K4" t="s">
-        <v>42</v>
-      </c>
       <c r="L4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="M4" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="N4" s="6"/>
       <c r="O4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="P4" t="str">
+        <v>63</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q4" t="str">
         <f t="shared" si="0"/>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="Q4" t="b">
+      <c r="R4" t="b">
         <v>1</v>
       </c>
-      <c r="R4" t="str">
+      <c r="S4" t="str">
         <f t="shared" si="1"/>
         <v>US</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>drstrange</v>
@@ -1272,30 +1356,33 @@
         <v>27</v>
       </c>
       <c r="L5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="N5" s="6" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="P5" t="str">
+        <v>63</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q5" t="str">
         <f t="shared" si="0"/>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="Q5" t="b">
+      <c r="R5" t="b">
         <v>1</v>
       </c>
-      <c r="R5" t="str">
+      <c r="S5" t="str">
         <f t="shared" si="1"/>
         <v>US</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>nursejazz</v>
@@ -1321,7 +1408,7 @@
         <v>29</v>
       </c>
       <c r="I6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J6" t="s">
         <v>26</v>
@@ -1330,28 +1417,33 @@
         <v>28</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="N6" s="6"/>
+        <v>78</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>82</v>
+      </c>
       <c r="O6" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="P6" t="str">
+        <v>85</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q6" t="str">
         <f t="shared" si="0"/>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="Q6" t="b">
+      <c r="R6" t="b">
         <v>1</v>
       </c>
-      <c r="R6" t="str">
+      <c r="S6" t="str">
         <f t="shared" si="1"/>
         <v>US</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="str">
         <f>SUBSTITUTE(LOWER(_xlfn.CONCAT(Table1[[#This Row],[Title]], Table1[[#This Row],[LastName]])), ".", "")</f>
         <v>nursesmith</v>
@@ -1385,43 +1477,48 @@
       <c r="K7" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="N7" s="6"/>
+      <c r="L7" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="O7" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="P7" t="str">
+        <v>85</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q7" t="str">
         <f t="shared" si="0"/>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="Q7" t="b">
+      <c r="R7" t="b">
         <v>1</v>
       </c>
-      <c r="R7" t="str">
+      <c r="S7" t="str">
         <f t="shared" si="1"/>
         <v>US</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="F8" s="15" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Title]], " ", Table1[[#This Row],[FirstName]], " ", Table1[[#This Row],[LastName]])</f>
@@ -1431,42 +1528,52 @@
         <v>16</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>23</v>
       </c>
       <c r="J8" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="K8" s="8" t="s">
-        <v>42</v>
-      </c>
       <c r="L8" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="N8" s="10"/>
+        <v>79</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>84</v>
+      </c>
       <c r="O8" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="P8" t="str">
+        <v>86</v>
+      </c>
+      <c r="P8" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q8" t="str">
         <f t="shared" si="0"/>
         <v>ENTERPRISEPREMIUM;EMSPREMIUM</v>
       </c>
-      <c r="Q8" t="b">
+      <c r="R8" t="b">
         <v>1</v>
       </c>
-      <c r="R8" t="str">
+      <c r="S8" t="str">
         <f t="shared" si="1"/>
         <v>US</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="A1:R1048576">
+  <conditionalFormatting sqref="A7:K7 M7:S7 A8:S1048576 A1:S6">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L7">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>

</xml_diff>